<commit_message>
se arreglo la url de puco y se hizo dinamica la seleccion de tabla
</commit_message>
<xml_diff>
--- a/static/mediaPOS/POS_HOAS10.xlsx
+++ b/static/mediaPOS/POS_HOAS10.xlsx
@@ -15,44 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">16669163    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CASTRO MONICA BEATRIZ         </t>
-  </si>
-  <si>
-    <t>O.S.P. SAN JUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16361773    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOLLATI ALEJANDRO HUMBERT     </t>
-  </si>
-  <si>
-    <t>O.S.P. CORDOBA (APOSS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50890703    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARISTI JUANA                  </t>
-  </si>
-  <si>
-    <t>O.S.P. BUENOS AIRES (IOMA) ; OBRA SOCIAL DE EJECUTIVOS Y DEL PERSONAL DE DIRECCION DE EMPRESAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27191653    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAVEZZA PABLO HERNAN          </t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DE LOS EMPLEADOS DE COMERCIO Y ACTIVIDADES CIVILES</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,52 +360,7 @@
     <col customWidth="1" max="2" min="2" width="35"/>
     <col customWidth="1" max="3" min="3" width="75"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>